<commit_message>
Hide nav bar on choosing entry. Fix some video names. Set page title to 'sensing evolution'.
</commit_message>
<xml_diff>
--- a/SensingEvolutionData.xlsx
+++ b/SensingEvolutionData.xlsx
@@ -6,21 +6,806 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Trails" sheetId="1" r:id="rId4"/>
-    <sheet name="Topics" sheetId="2" r:id="rId5"/>
-    <sheet name="Items" sheetId="3" r:id="rId6"/>
-    <sheet name="Questions" sheetId="4" r:id="rId7"/>
+    <sheet name="Info" sheetId="1" r:id="rId4"/>
+    <sheet name="Trails" sheetId="2" r:id="rId5"/>
+    <sheet name="Topics" sheetId="3" r:id="rId6"/>
+    <sheet name="Items" sheetId="4" r:id="rId7"/>
+    <sheet name="Questions" sheetId="5" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Sensing Evolution Data spreadsheet
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The pages of this spreadsheet together define the full dataset for the Sensing Evolution app.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Reference for all sheets and fields is allows:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Trails
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> - defines the trails which the user will be able to choose from
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">    - fields:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">        - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>slug.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> A unique identifier for the trail with no spaces
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">        - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">. The title of the trail seen by users
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">        - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>video</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>. The introductory video for this trail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Topics
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> - Defines the topics (groups of related items) which are in the exhibit. Topics can appear within any number of trails.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">   - fields:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">       - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>slug</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">. A unique identifier for each topic with no spaces
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">       - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">title. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The title of the topic seen by users
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">       - t</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">rail1, trail2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The slugs of trails to which this topic belongs. More columns can be added if a topic needs to belong to more than 2 trails. Leave trail2 blank if only 1 trail applies.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">       - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>fixed_order</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>. If this is ‘true’, all items in this topic will appear in the order they are in this spreadsheet. If ‘false’, they will be shuffled randomly.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Items
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">  - Defines the items in the exhibit. Items belong to a single topic, and can appear within any number of trails if multiple trails feature that topic.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">   - fields:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">      - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>slug</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">. Unique identifier for each item
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">      - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">. The title of the item seen by users
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">      - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">topic. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The slug of the topic to which this item belongs
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">      - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">trail1, trail2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The slugs of the trails on which the item should appear. More columns can be added if a topic needs to belong to more than 2 trails. Leave trail2 blank if only 1 trail applies.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">      - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">. The filename of the image to be shown on the items page. e.g. ‘megalosaurus.png’
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">      - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>video</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">. The filename of the video to be shown after finding this item.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">      - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>hint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">. The hint text to be shown when the user elects to view the hint for this item.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">      - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>beaconId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">. The Major ID of the iBeacon for this item
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">      - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">beaconHint. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">A hint seen only by developers/testers as to which beacon this is (e.g. purple)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Questions
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> - Defines the questions attached to each item. Questions belong to a single item and can apply to any number of trails. i.e. Multiple questions can have the same item field, but belong to different trails so that e.g. a harder question can be asked on the secondary school trail than on the primary school one. There can be only one question may be asked for a given item on a given trail.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">  - fields:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">    - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>slug:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> Unique identifier for the question
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">    - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">: slug of the item to which this question belongs
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">    - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">trail1, trail2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The slugs of trails on which this question should be asked.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">    - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">correctAnswer: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The text for the correct answer
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">    - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">correctResponse: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The response shown to the user after selecting the correct answer
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">    - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>incorrectAnswer1/2, incorrectResponse1/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">: The answer and response texts for the incorrect answers. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Note: All answers are shown in a different random order each time the question is asked.</t>
+    </r>
+  </si>
   <si>
     <t>slug</t>
   </si>
   <si>
-    <t>name</t>
+    <t>title</t>
+  </si>
+  <si>
+    <t>video</t>
   </si>
   <si>
     <t>primary-trail</t>
@@ -29,16 +814,22 @@
     <t>Primary School Trail</t>
   </si>
   <si>
+    <t>0. INTRODUCTION V2.mp4</t>
+  </si>
+  <si>
     <t>gcse-trail</t>
   </si>
   <si>
     <t>GCSE Trail</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>trail</t>
+    <t>trail1</t>
+  </si>
+  <si>
+    <t>trail2</t>
+  </si>
+  <si>
+    <t>fixed_order</t>
   </si>
   <si>
     <t>fossils</t>
@@ -59,7 +850,7 @@
     <t>Species</t>
   </si>
   <si>
-    <t>natural-selection</t>
+    <t>selection</t>
   </si>
   <si>
     <t>Natural selection</t>
@@ -71,9 +862,6 @@
     <t>image</t>
   </si>
   <si>
-    <t>video</t>
-  </si>
-  <si>
     <t>hint</t>
   </si>
   <si>
@@ -92,7 +880,7 @@
     <t>fossil1.jpg</t>
   </si>
   <si>
-    <t>video.mp4</t>
+    <t>3. Megalosaurus.mp4</t>
   </si>
   <si>
     <t>Look on the rear wall</t>
@@ -110,7 +898,7 @@
     <t>fossil2.jpg</t>
   </si>
   <si>
-    <t>video2.mp4</t>
+    <t>4. Icthyosaur.mp4</t>
   </si>
   <si>
     <t>Purple</t>
@@ -125,9 +913,6 @@
     <t>fossil3.jpg</t>
   </si>
   <si>
-    <t>blah.mp4</t>
-  </si>
-  <si>
     <t>Blue</t>
   </si>
   <si>
@@ -137,6 +922,9 @@
     <t>mutation1.jpg</t>
   </si>
   <si>
+    <t>1. Buckland Case.mp4</t>
+  </si>
+  <si>
     <t>mutation2</t>
   </si>
   <si>
@@ -146,18 +934,21 @@
     <t>mutation2.jpg</t>
   </si>
   <si>
+    <t>2. Hyaena Life on Earth display.mp4</t>
+  </si>
+  <si>
     <t>selection1</t>
   </si>
   <si>
     <t>Survival of the fittest</t>
   </si>
   <si>
-    <t>selection</t>
-  </si>
-  <si>
     <t>selection1.jpg</t>
   </si>
   <si>
+    <t>5. Peppered Moth and Snails Script.mp4</t>
+  </si>
+  <si>
     <t>selection2</t>
   </si>
   <si>
@@ -167,12 +958,18 @@
     <t>selection2.jpg</t>
   </si>
   <si>
+    <t>6. Darwin’s Pigeon Case Script.mp4</t>
+  </si>
+  <si>
     <t>species1</t>
   </si>
   <si>
     <t>species1.jpg</t>
   </si>
   <si>
+    <t>7. Reptiles SEvo Table.mp4</t>
+  </si>
+  <si>
     <t>species2</t>
   </si>
   <si>
@@ -182,6 +979,9 @@
     <t>species2.jpg</t>
   </si>
   <si>
+    <t>8. Archaeopteryx.mp4</t>
+  </si>
+  <si>
     <t>item</t>
   </si>
   <si>
@@ -264,6 +1064,9 @@
   </si>
   <si>
     <t>q-species1</t>
+  </si>
+  <si>
+    <t>q-species1-gcse</t>
   </si>
 </sst>
 </file>
@@ -273,7 +1076,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -305,6 +1108,13 @@
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <b val="1"/>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -315,18 +1125,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
+        <fgColor indexed="10"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -336,17 +1146,194 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -355,23 +1342,89 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -397,6 +1450,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -1630,40 +2684,140 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.875" style="1" customWidth="1"/>
-    <col min="3" max="256" width="9" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.25" style="1" customWidth="1"/>
+    <col min="8" max="256" width="12.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.55" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" ht="8" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" ht="20.55" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" ht="609.1" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" t="s" s="8">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" t="s" s="3">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" ht="20.35" customHeight="1">
-      <c r="A3" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" ht="20.35" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" ht="20.35" customHeight="1">
+      <c r="A6" s="5"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" ht="20.35" customHeight="1">
+      <c r="A7" s="5"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" ht="20.35" customHeight="1">
+      <c r="A8" s="5"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" ht="20.35" customHeight="1">
+      <c r="A9" s="5"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" ht="20.35" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" ht="20.35" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" ht="20.35" customHeight="1">
+      <c r="A12" s="5"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" ht="20.35" customHeight="1">
+      <c r="A13" s="10"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1679,72 +2833,107 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="5" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="5" customWidth="1"/>
-    <col min="4" max="256" width="12.25" style="5" customWidth="1"/>
+    <col min="1" max="1" width="9.125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="14.875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="18.0938" style="11" customWidth="1"/>
+    <col min="4" max="4" width="9" style="11" customWidth="1"/>
+    <col min="5" max="5" width="9" style="11" customWidth="1"/>
+    <col min="6" max="256" width="9" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.55" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="2">
+      <c r="A1" t="s" s="12">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s" s="12">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s" s="12">
+        <v>3</v>
+      </c>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" ht="20.55" customHeight="1">
+      <c r="A2" t="s" s="15">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s" s="8">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s" s="8">
         <v>6</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" ht="20.35" customHeight="1">
+      <c r="A3" t="s" s="15">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="B3" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="B2" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" ht="20.35" customHeight="1">
-      <c r="A3" t="s" s="3">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s" s="4">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s" s="4">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s" s="4">
-        <v>2</v>
-      </c>
+      <c r="C3" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="17"/>
+    </row>
+    <row r="4" ht="20" customHeight="1">
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" ht="20" customHeight="1">
+      <c r="A5" s="21"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" ht="20" customHeight="1">
+      <c r="A6" s="21"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" ht="20" customHeight="1">
+      <c r="A7" s="21"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="17"/>
+    </row>
+    <row r="8" ht="20" customHeight="1">
+      <c r="A8" s="21"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="17"/>
+    </row>
+    <row r="9" ht="20" customHeight="1">
+      <c r="A9" s="21"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" ht="20" customHeight="1">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1760,313 +2949,135 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12.25" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.25" style="6" customWidth="1"/>
-    <col min="7" max="7" width="12.25" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.25" style="6" customWidth="1"/>
-    <col min="9" max="9" width="12.25" style="6" customWidth="1"/>
-    <col min="10" max="256" width="12.25" style="6" customWidth="1"/>
+    <col min="1" max="1" width="12.25" style="25" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="25" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="25" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="25" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="25" customWidth="1"/>
+    <col min="6" max="256" width="12.25" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.55" customHeight="1">
-      <c r="A1" t="s" s="2">
+      <c r="A1" t="s" s="12">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s" s="12">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" ht="20.55" customHeight="1">
+      <c r="A2" t="s" s="15">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s" s="8">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="E2" t="b" s="26">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s" s="2">
+    </row>
+    <row r="3" ht="20.35" customHeight="1">
+      <c r="A3" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s" s="8">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="E3" t="b" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" ht="20.35" customHeight="1">
+      <c r="A4" t="s" s="15">
         <v>16</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="B4" t="s" s="8">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="E1" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s" s="2">
+      <c r="D4" s="9"/>
+      <c r="E4" t="b" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="A5" t="s" s="15">
         <v>18</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="B5" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="H1" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" ht="32.55" customHeight="1">
-      <c r="A2" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s" s="4">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s" s="4">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s" s="4">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s" s="4">
-        <v>26</v>
-      </c>
-      <c r="H2" s="4">
-        <v>6650</v>
-      </c>
-      <c r="I2" t="s" s="4">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" ht="20.35" customHeight="1">
-      <c r="A3" t="s" s="3">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s" s="4">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s" s="4">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s" s="4">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s" s="4">
-        <v>19</v>
-      </c>
-      <c r="H3" s="4">
-        <v>45790</v>
-      </c>
-      <c r="I3" t="s" s="4">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="3">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s" s="4">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s" s="4">
-        <v>35</v>
-      </c>
-      <c r="F4" t="s" s="4">
-        <v>36</v>
-      </c>
-      <c r="G4" t="s" s="4">
-        <v>19</v>
-      </c>
-      <c r="H4" s="4">
-        <v>26981</v>
-      </c>
-      <c r="I4" t="s" s="4">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" t="s" s="3">
-        <v>38</v>
-      </c>
-      <c r="B5" t="s" s="4">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s" s="4">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s" s="4">
-        <v>39</v>
-      </c>
-      <c r="F5" t="s" s="4">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s" s="4">
-        <v>19</v>
-      </c>
-      <c r="H5" s="4">
-        <v>45790</v>
-      </c>
-      <c r="I5" t="s" s="4">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" t="s" s="3">
-        <v>40</v>
-      </c>
-      <c r="B6" t="s" s="4">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s" s="4">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s" s="4">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s" s="4">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s" s="4">
-        <v>19</v>
-      </c>
-      <c r="H6" s="4">
-        <v>26981</v>
-      </c>
-      <c r="I6" t="s" s="4">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" ht="32.35" customHeight="1">
-      <c r="A7" t="s" s="3">
-        <v>43</v>
-      </c>
-      <c r="B7" t="s" s="4">
-        <v>44</v>
-      </c>
-      <c r="C7" t="s" s="4">
-        <v>45</v>
-      </c>
-      <c r="D7" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s" s="4">
-        <v>46</v>
-      </c>
-      <c r="F7" t="s" s="4">
-        <v>25</v>
-      </c>
-      <c r="G7" t="s" s="4">
-        <v>19</v>
-      </c>
-      <c r="H7" s="4">
-        <v>6650</v>
-      </c>
-      <c r="I7" t="s" s="4">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" t="s" s="3">
-        <v>47</v>
-      </c>
-      <c r="B8" t="s" s="4">
-        <v>48</v>
-      </c>
-      <c r="C8" t="s" s="4">
-        <v>45</v>
-      </c>
-      <c r="D8" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s" s="4">
-        <v>49</v>
-      </c>
-      <c r="F8" t="s" s="4">
-        <v>25</v>
-      </c>
-      <c r="G8" t="s" s="4">
-        <v>19</v>
-      </c>
-      <c r="H8" s="4">
-        <v>45790</v>
-      </c>
-      <c r="I8" t="s" s="4">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" t="s" s="3">
-        <v>50</v>
-      </c>
-      <c r="B9" t="s" s="4">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E9" t="s" s="4">
-        <v>51</v>
-      </c>
-      <c r="F9" t="s" s="4">
-        <v>25</v>
-      </c>
-      <c r="G9" t="s" s="4">
-        <v>19</v>
-      </c>
-      <c r="H9" s="4">
-        <v>6650</v>
-      </c>
-      <c r="I9" t="s" s="4">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" t="s" s="3">
-        <v>52</v>
-      </c>
-      <c r="B10" t="s" s="4">
-        <v>53</v>
-      </c>
-      <c r="C10" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s" s="4">
-        <v>54</v>
-      </c>
-      <c r="F10" t="s" s="4">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s" s="4">
-        <v>19</v>
-      </c>
-      <c r="H10" s="4">
-        <v>26981</v>
-      </c>
-      <c r="I10" t="s" s="4">
-        <v>37</v>
-      </c>
+      <c r="C5" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" t="b" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1">
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" ht="20" customHeight="1">
+      <c r="A7" s="21"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="17"/>
+    </row>
+    <row r="8" ht="20" customHeight="1">
+      <c r="A8" s="21"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="17"/>
+    </row>
+    <row r="9" ht="20" customHeight="1">
+      <c r="A9" s="21"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" ht="20" customHeight="1">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2082,375 +3093,804 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="7" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="7" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="7" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="7" customWidth="1"/>
-    <col min="5" max="5" width="12.25" style="7" customWidth="1"/>
-    <col min="6" max="6" width="24.5" style="7" customWidth="1"/>
-    <col min="7" max="7" width="12.25" style="7" customWidth="1"/>
-    <col min="8" max="8" width="27.875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="27.25" style="7" customWidth="1"/>
-    <col min="11" max="256" width="12.25" style="7" customWidth="1"/>
+    <col min="1" max="1" width="12.25" style="28" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="28" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="28" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="28" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="28" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="28" customWidth="1"/>
+    <col min="7" max="7" width="21.6406" style="28" customWidth="1"/>
+    <col min="8" max="8" width="12.25" style="28" customWidth="1"/>
+    <col min="9" max="9" width="12.25" style="28" customWidth="1"/>
+    <col min="10" max="10" width="12.25" style="28" customWidth="1"/>
+    <col min="11" max="256" width="12.25" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.55" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="2">
+      <c r="A1" t="s" s="12">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s" s="12">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s" s="12">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s" s="12">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s" s="12">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s" s="12">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s" s="12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" ht="32.55" customHeight="1">
+      <c r="A2" t="s" s="15">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s" s="8">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s" s="8">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s" s="8">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s" s="8">
+        <v>29</v>
+      </c>
+      <c r="I2" s="8">
+        <v>6650</v>
+      </c>
+      <c r="J2" t="s" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" ht="20.35" customHeight="1">
+      <c r="A3" t="s" s="15">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s" s="8">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s" s="8">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s" s="8">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s" s="8">
+        <v>22</v>
+      </c>
+      <c r="I3" s="8">
+        <v>45790</v>
+      </c>
+      <c r="J3" t="s" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" ht="20.35" customHeight="1">
+      <c r="A4" t="s" s="15">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s" s="8">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s" s="8">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" t="s" s="8">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s" s="8">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s" s="8">
+        <v>22</v>
+      </c>
+      <c r="I4" s="8">
+        <v>26981</v>
+      </c>
+      <c r="J4" t="s" s="8">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="A5" t="s" s="15">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s" s="8">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s" s="8">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s" s="8">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s" s="8">
+        <v>22</v>
+      </c>
+      <c r="I5" s="8">
+        <v>45790</v>
+      </c>
+      <c r="J5" t="s" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" ht="20.35" customHeight="1">
+      <c r="A6" t="s" s="15">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s" s="8">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s" s="8">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s" s="8">
+        <v>46</v>
+      </c>
+      <c r="H6" t="s" s="8">
+        <v>22</v>
+      </c>
+      <c r="I6" s="8">
+        <v>26981</v>
+      </c>
+      <c r="J6" t="s" s="8">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" ht="32.35" customHeight="1">
+      <c r="A7" t="s" s="15">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s" s="8">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s" s="8">
+        <v>49</v>
+      </c>
+      <c r="G7" t="s" s="8">
+        <v>50</v>
+      </c>
+      <c r="H7" t="s" s="8">
+        <v>22</v>
+      </c>
+      <c r="I7" s="8">
+        <v>6650</v>
+      </c>
+      <c r="J7" t="s" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" ht="20.35" customHeight="1">
+      <c r="A8" t="s" s="15">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s" s="8">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" t="s" s="8">
+        <v>53</v>
+      </c>
+      <c r="G8" t="s" s="8">
+        <v>54</v>
+      </c>
+      <c r="H8" t="s" s="8">
+        <v>22</v>
+      </c>
+      <c r="I8" s="8">
+        <v>45790</v>
+      </c>
+      <c r="J8" t="s" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" ht="20.35" customHeight="1">
+      <c r="A9" t="s" s="15">
         <v>55</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="B9" t="s" s="8">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="F9" t="s" s="8">
         <v>56</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="G9" t="s" s="8">
         <v>57</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="H9" t="s" s="8">
+        <v>22</v>
+      </c>
+      <c r="I9" s="8">
+        <v>6650</v>
+      </c>
+      <c r="J9" t="s" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" ht="20.35" customHeight="1">
+      <c r="A10" t="s" s="15">
         <v>58</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="B10" t="s" s="8">
         <v>59</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="C10" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" t="s" s="8">
         <v>60</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="G10" t="s" s="8">
         <v>61</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="H10" t="s" s="8">
+        <v>22</v>
+      </c>
+      <c r="I10" s="8">
+        <v>26981</v>
+      </c>
+      <c r="J10" t="s" s="8">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="12.25" style="29" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="29" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="29" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="29" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="29" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="29" customWidth="1"/>
+    <col min="7" max="7" width="24.5" style="29" customWidth="1"/>
+    <col min="8" max="8" width="12.25" style="29" customWidth="1"/>
+    <col min="9" max="9" width="27.875" style="29" customWidth="1"/>
+    <col min="10" max="10" width="13.625" style="29" customWidth="1"/>
+    <col min="11" max="11" width="27.25" style="29" customWidth="1"/>
+    <col min="12" max="256" width="12.25" style="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20.55" customHeight="1">
+      <c r="A1" t="s" s="12">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s" s="12">
         <v>62</v>
       </c>
+      <c r="C1" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s" s="12">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s" s="12">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s" s="12">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s" s="12">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s" s="12">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s" s="12">
+        <v>68</v>
+      </c>
+      <c r="K1" t="s" s="12">
+        <v>69</v>
+      </c>
     </row>
     <row r="2" ht="92.55" customHeight="1">
-      <c r="A2" t="s" s="3">
-        <v>63</v>
-      </c>
-      <c r="B2" t="s" s="4">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s" s="4">
-        <v>64</v>
-      </c>
-      <c r="E2" t="s" s="4">
-        <v>65</v>
-      </c>
-      <c r="F2" t="s" s="4">
-        <v>66</v>
-      </c>
-      <c r="G2" t="s" s="4">
-        <v>67</v>
-      </c>
-      <c r="H2" t="s" s="4">
-        <v>68</v>
-      </c>
-      <c r="I2" t="s" s="4">
-        <v>69</v>
-      </c>
-      <c r="J2" t="s" s="4">
+      <c r="A2" t="s" s="15">
         <v>70</v>
       </c>
+      <c r="B2" t="s" s="8">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="F2" t="s" s="8">
+        <v>72</v>
+      </c>
+      <c r="G2" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="H2" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="I2" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="J2" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="K2" t="s" s="8">
+        <v>77</v>
+      </c>
     </row>
     <row r="3" ht="92.35" customHeight="1">
-      <c r="A3" t="s" s="3">
+      <c r="A3" t="s" s="15">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s" s="8">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" t="s" s="8">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s" s="8">
+        <v>80</v>
+      </c>
+      <c r="G3" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="H3" t="s" s="8">
+        <v>81</v>
+      </c>
+      <c r="I3" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="J3" t="s" s="8">
+        <v>82</v>
+      </c>
+      <c r="K3" t="s" s="8">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" ht="92.35" customHeight="1">
+      <c r="A4" t="s" s="15">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s" s="8">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" t="s" s="8">
         <v>71</v>
       </c>
-      <c r="B3" t="s" s="4">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s" s="4">
+      <c r="F4" t="s" s="8">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="I4" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="J4" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="K4" t="s" s="8">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" ht="92.35" customHeight="1">
+      <c r="A5" t="s" s="15">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s" s="8">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="F5" t="s" s="8">
+        <v>72</v>
+      </c>
+      <c r="G5" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="H5" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="I5" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="J5" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="K5" t="s" s="8">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" ht="92.35" customHeight="1">
+      <c r="A6" t="s" s="15">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s" s="8">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s" s="8">
         <v>4</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="D6" s="9"/>
+      <c r="E6" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="F6" t="s" s="8">
         <v>72</v>
       </c>
-      <c r="E3" t="s" s="4">
+      <c r="G6" t="s" s="8">
         <v>73</v>
       </c>
-      <c r="F3" t="s" s="4">
-        <v>66</v>
-      </c>
-      <c r="G3" t="s" s="4">
+      <c r="H6" t="s" s="8">
         <v>74</v>
       </c>
-      <c r="H3" t="s" s="4">
-        <v>68</v>
-      </c>
-      <c r="I3" t="s" s="4">
+      <c r="I6" t="s" s="8">
         <v>75</v>
       </c>
-      <c r="J3" t="s" s="4">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" ht="92.35" customHeight="1">
-      <c r="A4" t="s" s="3">
+      <c r="J6" t="s" s="8">
         <v>76</v>
       </c>
-      <c r="B4" t="s" s="4">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s" s="4">
-        <v>64</v>
-      </c>
-      <c r="E4" t="s" s="4">
-        <v>65</v>
-      </c>
-      <c r="F4" t="s" s="4">
-        <v>66</v>
-      </c>
-      <c r="G4" t="s" s="4">
-        <v>67</v>
-      </c>
-      <c r="H4" t="s" s="4">
-        <v>68</v>
-      </c>
-      <c r="I4" t="s" s="4">
-        <v>69</v>
-      </c>
-      <c r="J4" t="s" s="4">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" ht="92.35" customHeight="1">
-      <c r="A5" t="s" s="3">
+      <c r="K6" t="s" s="8">
         <v>77</v>
       </c>
-      <c r="B5" t="s" s="4">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s" s="4">
-        <v>64</v>
-      </c>
-      <c r="E5" t="s" s="4">
-        <v>65</v>
-      </c>
-      <c r="F5" t="s" s="4">
-        <v>66</v>
-      </c>
-      <c r="G5" t="s" s="4">
-        <v>67</v>
-      </c>
-      <c r="H5" t="s" s="4">
-        <v>68</v>
-      </c>
-      <c r="I5" t="s" s="4">
-        <v>69</v>
-      </c>
-      <c r="J5" t="s" s="4">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" ht="92.35" customHeight="1">
-      <c r="A6" t="s" s="3">
-        <v>78</v>
-      </c>
-      <c r="B6" t="s" s="4">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s" s="4">
-        <v>64</v>
-      </c>
-      <c r="E6" t="s" s="4">
-        <v>65</v>
-      </c>
-      <c r="F6" t="s" s="4">
-        <v>66</v>
-      </c>
-      <c r="G6" t="s" s="4">
-        <v>67</v>
-      </c>
-      <c r="H6" t="s" s="4">
-        <v>68</v>
-      </c>
-      <c r="I6" t="s" s="4">
-        <v>69</v>
-      </c>
-      <c r="J6" t="s" s="4">
-        <v>70</v>
-      </c>
     </row>
     <row r="7" ht="92.35" customHeight="1">
-      <c r="A7" t="s" s="3">
-        <v>79</v>
-      </c>
-      <c r="B7" t="s" s="4">
+      <c r="A7" t="s" s="15">
+        <v>85</v>
+      </c>
+      <c r="B7" t="s" s="8">
         <v>40</v>
       </c>
-      <c r="C7" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s" s="4">
-        <v>64</v>
-      </c>
-      <c r="E7" t="s" s="4">
-        <v>65</v>
-      </c>
-      <c r="F7" t="s" s="4">
-        <v>66</v>
-      </c>
-      <c r="G7" t="s" s="4">
-        <v>67</v>
-      </c>
-      <c r="H7" t="s" s="4">
-        <v>68</v>
-      </c>
-      <c r="I7" t="s" s="4">
-        <v>69</v>
-      </c>
-      <c r="J7" t="s" s="4">
-        <v>70</v>
+      <c r="C7" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="F7" t="s" s="8">
+        <v>72</v>
+      </c>
+      <c r="G7" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="H7" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="I7" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="J7" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="K7" t="s" s="8">
+        <v>77</v>
       </c>
     </row>
     <row r="8" ht="92.35" customHeight="1">
-      <c r="A8" t="s" s="3">
-        <v>80</v>
-      </c>
-      <c r="B8" t="s" s="4">
+      <c r="A8" t="s" s="15">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s" s="8">
         <v>43</v>
       </c>
-      <c r="C8" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s" s="4">
-        <v>64</v>
-      </c>
-      <c r="E8" t="s" s="4">
-        <v>65</v>
-      </c>
-      <c r="F8" t="s" s="4">
-        <v>66</v>
-      </c>
-      <c r="G8" t="s" s="4">
-        <v>67</v>
-      </c>
-      <c r="H8" t="s" s="4">
-        <v>68</v>
-      </c>
-      <c r="I8" t="s" s="4">
-        <v>69</v>
-      </c>
-      <c r="J8" t="s" s="4">
-        <v>70</v>
+      <c r="C8" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="F8" t="s" s="8">
+        <v>72</v>
+      </c>
+      <c r="G8" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="H8" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="I8" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="J8" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="K8" t="s" s="8">
+        <v>77</v>
       </c>
     </row>
     <row r="9" ht="92.35" customHeight="1">
-      <c r="A9" t="s" s="3">
-        <v>81</v>
-      </c>
-      <c r="B9" t="s" s="4">
+      <c r="A9" t="s" s="15">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s" s="8">
         <v>47</v>
       </c>
-      <c r="C9" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s" s="4">
-        <v>64</v>
-      </c>
-      <c r="E9" t="s" s="4">
-        <v>65</v>
-      </c>
-      <c r="F9" t="s" s="4">
-        <v>66</v>
-      </c>
-      <c r="G9" t="s" s="4">
-        <v>67</v>
-      </c>
-      <c r="H9" t="s" s="4">
-        <v>68</v>
-      </c>
-      <c r="I9" t="s" s="4">
-        <v>69</v>
-      </c>
-      <c r="J9" t="s" s="4">
-        <v>70</v>
+      <c r="C9" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="F9" t="s" s="8">
+        <v>72</v>
+      </c>
+      <c r="G9" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="H9" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="I9" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="J9" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="K9" t="s" s="8">
+        <v>77</v>
       </c>
     </row>
     <row r="10" ht="92.35" customHeight="1">
-      <c r="A10" t="s" s="3">
-        <v>82</v>
-      </c>
-      <c r="B10" t="s" s="4">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s" s="4">
-        <v>64</v>
-      </c>
-      <c r="E10" t="s" s="4">
-        <v>65</v>
-      </c>
-      <c r="F10" t="s" s="4">
-        <v>66</v>
-      </c>
-      <c r="G10" t="s" s="4">
-        <v>67</v>
-      </c>
-      <c r="H10" t="s" s="4">
-        <v>68</v>
-      </c>
-      <c r="I10" t="s" s="4">
-        <v>69</v>
-      </c>
-      <c r="J10" t="s" s="4">
-        <v>70</v>
+      <c r="A10" t="s" s="15">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s" s="8">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="F10" t="s" s="8">
+        <v>72</v>
+      </c>
+      <c r="G10" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="H10" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="I10" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="J10" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="K10" t="s" s="8">
+        <v>77</v>
       </c>
     </row>
     <row r="11" ht="92.35" customHeight="1">
-      <c r="A11" t="s" s="3">
-        <v>82</v>
-      </c>
-      <c r="B11" t="s" s="4">
-        <v>52</v>
-      </c>
-      <c r="C11" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s" s="4">
-        <v>64</v>
-      </c>
-      <c r="E11" t="s" s="4">
-        <v>65</v>
-      </c>
-      <c r="F11" t="s" s="4">
-        <v>66</v>
-      </c>
-      <c r="G11" t="s" s="4">
-        <v>67</v>
-      </c>
-      <c r="H11" t="s" s="4">
-        <v>68</v>
-      </c>
-      <c r="I11" t="s" s="4">
-        <v>69</v>
-      </c>
-      <c r="J11" t="s" s="4">
-        <v>70</v>
+      <c r="A11" t="s" s="15">
+        <v>89</v>
+      </c>
+      <c r="B11" t="s" s="8">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="F11" t="s" s="8">
+        <v>72</v>
+      </c>
+      <c r="G11" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="H11" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="I11" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="J11" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="K11" t="s" s="8">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" ht="92.35" customHeight="1">
+      <c r="A12" t="s" s="15">
+        <v>90</v>
+      </c>
+      <c r="B12" t="s" s="8">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="F12" t="s" s="8">
+        <v>72</v>
+      </c>
+      <c r="G12" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="H12" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="I12" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="J12" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="K12" t="s" s="8">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" ht="92.35" customHeight="1">
+      <c r="A13" t="s" s="15">
+        <v>89</v>
+      </c>
+      <c r="B13" t="s" s="8">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="F13" t="s" s="8">
+        <v>72</v>
+      </c>
+      <c r="G13" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="H13" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="I13" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="J13" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="K13" t="s" s="8">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>